<commit_message>
Commit of final Cannabis notebook to manny branch
</commit_message>
<xml_diff>
--- a/manny/Data/US_market_byCategory_size.xlsx
+++ b/manny/Data/US_market_byCategory_size.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bxprd\Data Analytics Bootcamp\Git_Repos\data-analysis-project-1\manny\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC7E49DF-4D8A-4B19-93C7-7DF1970D0C75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD40693E-E1D7-4496-95DA-BC0B7A76EF30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US_market_byCategory_size" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">US_market_byCategory_size!$A$1:$I$217</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -79,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -914,11 +917,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I217"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="M78" sqref="M78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,7 +929,7 @@
     <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -954,8 +957,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -983,8 +989,11 @@
       <c r="I2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43497</v>
       </c>
@@ -1012,8 +1021,11 @@
       <c r="I3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43525</v>
       </c>
@@ -1041,8 +1053,11 @@
       <c r="I4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43556</v>
       </c>
@@ -1070,8 +1085,11 @@
       <c r="I5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43586</v>
       </c>
@@ -1099,8 +1117,11 @@
       <c r="I6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43617</v>
       </c>
@@ -1128,8 +1149,11 @@
       <c r="I7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43647</v>
       </c>
@@ -1157,8 +1181,11 @@
       <c r="I8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43678</v>
       </c>
@@ -1186,8 +1213,11 @@
       <c r="I9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43709</v>
       </c>
@@ -1215,8 +1245,11 @@
       <c r="I10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43739</v>
       </c>
@@ -1245,7 +1278,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43770</v>
       </c>
@@ -1274,7 +1307,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43800</v>
       </c>
@@ -1303,7 +1336,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43831</v>
       </c>
@@ -1332,7 +1365,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43862</v>
       </c>
@@ -1361,7 +1394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43891</v>
       </c>
@@ -7220,6 +7253,8 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I217" xr:uid="{AC07E126-E80E-4369-9AF3-DF05622450D5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>